<commit_message>
fr inpatient to fr patinet 01457e066567c6e3959b08caf1bf81e6ef52764d
</commit_message>
<xml_diff>
--- a/nr-review/ig/PN13-FHIR-prescmed-encounter-conceptmap.xlsx
+++ b/nr-review/ig/PN13-FHIR-prescmed-encounter-conceptmap.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-11T13:00:29+00:00</t>
+    <t>2025-07-15T07:25:49+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -99,7 +99,7 @@
     <t>Target</t>
   </si>
   <si>
-    <t>https://hl7.fr/ig/fhir/medication/StructureDefinition/fr-inpatient-medicationrequest</t>
+    <t>https://hl7.fr/ig/fhir/medication/StructureDefinition/fr-patient-medicationrequest</t>
   </si>
   <si>
     <t>Display</t>

</xml_diff>

<commit_message>
Revert "update profile names"
This reverts commit 794f8ff8dd4ea40db45888cea7176d3247b22ccc. d63c4208035ef6f3e0a52345f6867c3ff9f32776
</commit_message>
<xml_diff>
--- a/nr-review/ig/PN13-FHIR-prescmed-encounter-conceptmap.xlsx
+++ b/nr-review/ig/PN13-FHIR-prescmed-encounter-conceptmap.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-18T11:27:43+00:00</t>
+    <t>2025-07-18T11:28:48+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -99,7 +99,7 @@
     <t>Target</t>
   </si>
   <si>
-    <t>https://hl7.fr/ig/fhir/medication/StructureDefinition/fr-inpatient-medicationrequest</t>
+    <t>https://hl7.fr/ig/fhir/medication/StructureDefinition/fr-patient-medicationrequest</t>
   </si>
   <si>
     <t>Display</t>

</xml_diff>